<commit_message>
Cleaned Up Directory + Deliverables
</commit_message>
<xml_diff>
--- a/TabulatedModelResults.xlsx
+++ b/TabulatedModelResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MastersRepos\Deep-Learning-For-Computer-Vision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995B8382-5A0C-4719-ACC6-122246D95003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FE5720-02C7-4F00-B07D-1FE64EED3FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E0EA7199-BBBF-4681-AB86-0D95C3B6BA8D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
   <si>
     <t>Source Dataset</t>
   </si>
@@ -78,6 +78,54 @@
   </si>
   <si>
     <t>https://chatgpt.com/c/6807b1bf-d978-8004-9a34-0e504258affb</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>11hr (132 Epochs)</t>
+  </si>
+  <si>
+    <t>14hr (111 Epochs)</t>
+  </si>
+  <si>
+    <t>2hr (63 Epochs)</t>
+  </si>
+  <si>
+    <t>11hr (68 Epochs)</t>
+  </si>
+  <si>
+    <t>4hr (50 Epochs)</t>
+  </si>
+  <si>
+    <t>6hr 30m (34 Epochs)</t>
+  </si>
+  <si>
+    <t>3hr 30m (81 Epochs)</t>
+  </si>
+  <si>
+    <t>15hr (99 Epochs)</t>
+  </si>
+  <si>
+    <t>15hr (145 Epochs)</t>
+  </si>
+  <si>
+    <t>2hr 30m (50 Epochs)</t>
+  </si>
+  <si>
+    <t>1hr (51 Epochs)</t>
+  </si>
+  <si>
+    <t>2hr (19 Epochs)</t>
+  </si>
+  <si>
+    <t>2hr (76 Epochs)</t>
+  </si>
+  <si>
+    <t>1hr (81 Epochs)</t>
+  </si>
+  <si>
+    <t>2hr (47 Epochs)</t>
   </si>
 </sst>
 </file>
@@ -160,12 +208,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,58 +548,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994FC9B0-781B-4386-9CEC-849C57C98C66}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>51.8</v>
       </c>
       <c r="C3">
@@ -566,15 +643,33 @@
       <c r="F3">
         <v>61.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4">
         <v>35.799999999999997</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>80.2</v>
       </c>
       <c r="D4">
@@ -589,8 +684,26 @@
       <c r="H4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -600,7 +713,7 @@
       <c r="C5">
         <v>55.7</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>60.9</v>
       </c>
       <c r="E5">
@@ -609,44 +722,62 @@
       <c r="F5">
         <v>74.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>61</v>
       </c>
       <c r="C10">
@@ -662,14 +793,14 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11">
         <v>46.9</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>88.8</v>
       </c>
       <c r="D11">
@@ -682,7 +813,7 @@
         <v>82.8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -692,7 +823,7 @@
       <c r="C12">
         <v>45.8</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>70.099999999999994</v>
       </c>
       <c r="E12">
@@ -702,35 +833,35 @@
         <v>81.7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -738,7 +869,7 @@
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>58.7</v>
       </c>
       <c r="C17">
@@ -761,7 +892,7 @@
       <c r="B18">
         <v>41.1</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>78</v>
       </c>
       <c r="D18">
@@ -784,7 +915,7 @@
       <c r="C19">
         <v>64.099999999999994</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>68</v>
       </c>
       <c r="E19">
@@ -798,31 +929,31 @@
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -830,7 +961,7 @@
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>56</v>
       </c>
       <c r="C24">
@@ -853,7 +984,7 @@
       <c r="B25">
         <v>43.7</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>83.3</v>
       </c>
       <c r="D25">
@@ -876,7 +1007,7 @@
       <c r="C26">
         <v>63.9</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <v>67.3</v>
       </c>
       <c r="E26">
@@ -890,31 +1021,31 @@
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -922,7 +1053,7 @@
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>48.4</v>
       </c>
       <c r="C31">
@@ -945,7 +1076,7 @@
       <c r="B32">
         <v>32.200000000000003</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>78.099999999999994</v>
       </c>
       <c r="D32">
@@ -968,7 +1099,7 @@
       <c r="C33">
         <v>58</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="4">
         <v>62.4</v>
       </c>
       <c r="E33">
@@ -979,12 +1110,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="K1:O1"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>